<commit_message>
Atualização do Arquivo .xlsx
</commit_message>
<xml_diff>
--- a/Processo de Criação do Diretório.xlsx
+++ b/Processo de Criação do Diretório.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0200832311026\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0200832311026\Desktop\A1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Passo</t>
   </si>
@@ -89,13 +89,22 @@
     <t>As alterações realizadas no ramo foram salvas.</t>
   </si>
   <si>
-    <t>git push origin main</t>
-  </si>
-  <si>
-    <t>Realizado o Pull Request pelo github</t>
-  </si>
-  <si>
-    <t>Integração do site no Github.</t>
+    <t>git checkout main</t>
+  </si>
+  <si>
+    <t>Retornado para o ramo principal.</t>
+  </si>
+  <si>
+    <t>git push origin admin</t>
+  </si>
+  <si>
+    <t>Os arquivos do ramo foram adicionados ao repositório do Github.</t>
+  </si>
+  <si>
+    <t>Realizado o Pull Request pelo Github</t>
+  </si>
+  <si>
+    <t>Adicionado o ramo admin no Github.</t>
   </si>
 </sst>
 </file>
@@ -248,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,13 +286,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -566,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,11 +730,11 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>17</v>
+      <c r="C13" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,11 +742,32 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="12" t="s">
         <v>23</v>
       </c>
+      <c r="C14" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>14</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>